<commit_message>
Abandoned oCamS for ZED Mini and updated Glue Board
Abandoned oCamS for ZED Mini and updated Glue Board
</commit_message>
<xml_diff>
--- a/Electronics/Glue Board/Glue_Board_BOM.xlsx
+++ b/Electronics/Glue Board/Glue_Board_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arko/GitHub/robocar-pinky/Electronics/Glue Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{920A674B-C4D1-434A-B1D2-B4C647A109C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E0C26F-16B9-AF46-8488-ED32D0E58851}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29000" yWindow="-10860" windowWidth="41200" windowHeight="22580" xr2:uid="{EB2B9FEF-4548-A944-A3FC-D1BA110BF293}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{EB2B9FEF-4548-A944-A3FC-D1BA110BF293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{4C0866A3-78DA-7A4E-969D-37A29354A642}" name="Glue Board" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/arko/GitHub/robocar-pinky/Electronics/Glue Board/Glue Board.csv" comma="1" semicolon="1">
+    <textPr sourceFile="/Users/arko/GitHub/robocar-pinky/Electronics/Glue Board/Glue Board.csv" comma="1" semicolon="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="154">
   <si>
     <t>Reference</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>INA260AIPW</t>
+  </si>
+  <si>
+    <t>PCA9685PW/Q900,118</t>
   </si>
 </sst>
 </file>
@@ -866,7 +869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38993CA9-71F4-C045-9E02-F61913B15C94}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1586,7 +1591,7 @@
         <v>121</v>
       </c>
       <c r="F36" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added harnessing and assembly diagrams
Added harnessing and assembly diagrams
</commit_message>
<xml_diff>
--- a/Electronics/Glue Board/Glue_Board_BOM.xlsx
+++ b/Electronics/Glue Board/Glue_Board_BOM.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arko/GitHub/robocar-pinky/Electronics/Glue Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E0C26F-16B9-AF46-8488-ED32D0E58851}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5321E269-F1F3-A94E-B98E-0C4E9447BF09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{EB2B9FEF-4548-A944-A3FC-D1BA110BF293}"/>
+    <workbookView xWindow="35840" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{EB2B9FEF-4548-A944-A3FC-D1BA110BF293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Glue_Board" localSheetId="0">Sheet1!$A$1:$F$43</definedName>
+    <definedName name="Glue_Board" localSheetId="0">Sheet1!$A$1:$F$45</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="158">
   <si>
     <t>Reference</t>
   </si>
@@ -151,9 +151,6 @@
     <t>agg:DO-214AB-SMC</t>
   </si>
   <si>
-    <t xml:space="preserve">D2 D3 </t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>ESR03EZPJ470</t>
   </si>
   <si>
-    <t xml:space="preserve">SW1 SW2 </t>
-  </si>
-  <si>
     <t>SW_SPST</t>
   </si>
   <si>
@@ -512,6 +506,24 @@
   </si>
   <si>
     <t>PCA9685PW/Q900,118</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3 </t>
+  </si>
+  <si>
+    <t>MPR3RD</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>M2011LL1W01-C</t>
   </si>
 </sst>
 </file>
@@ -547,8 +559,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38993CA9-71F4-C045-9E02-F61913B15C94}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,673 +1080,713 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="F16">
-        <v>530470510</v>
+      <c r="F16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
+      </c>
+      <c r="F17" s="1">
+        <v>530470510</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
-      </c>
-      <c r="F18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>470</v>
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
       </c>
       <c r="D23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
         <v>79</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B24">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>470</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
         <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
         <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E37" t="s">
-        <v>125</v>
-      </c>
-      <c r="F37" t="s">
-        <v>126</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E38" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F38" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E39" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F39" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E40" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F40" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D41" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F41" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F42" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" t="s">
+        <v>142</v>
+      </c>
+      <c r="F43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" t="s">
+        <v>145</v>
+      </c>
+      <c r="E44" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" t="s">
         <v>148</v>
       </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="E45" t="s">
         <v>149</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F45" t="s">
         <v>150</v>
-      </c>
-      <c r="E43" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>